<commit_message>
Swapped caseitem_note for person_not as per IN-414. Also added a janky test and a type as per IN-410
</commit_message>
<xml_diff>
--- a/etl2/docs/mapping_doc.xlsx
+++ b/etl2/docs/mapping_doc.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jennifermackown/Documents/MOJ/opg-data-casrec-migration/etl2/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0110CDAB-5900-CC48-A330-7F11B0EACFC1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17B31E55-392B-BA41-B31B-196873E26B08}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22940" yWindow="460" windowWidth="45860" windowHeight="28340" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="22920" windowHeight="28340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="persons (Client)" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="900" uniqueCount="306">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="900" uniqueCount="305">
   <si>
     <t>column_name</t>
   </si>
@@ -648,9 +648,6 @@
     <t>default_value</t>
   </si>
   <si>
-    <t>default_string</t>
-  </si>
-  <si>
     <t>is_pk</t>
   </si>
   <si>
@@ -1032,7 +1029,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1063,6 +1060,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1137,7 +1140,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -1159,6 +1162,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1376,9 +1380,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U1000"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="T17" sqref="T17"/>
+      <selection pane="bottomLeft" activeCell="U19" sqref="U19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1410,7 +1414,7 @@
         <v>6</v>
       </c>
       <c r="H1" s="8" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="I1" s="8" t="s">
         <v>7</v>
@@ -1754,7 +1758,7 @@
         <v>0</v>
       </c>
       <c r="T17" s="6" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="18" spans="1:21" ht="14" x14ac:dyDescent="0.15">
@@ -1773,8 +1777,8 @@
       <c r="G18" s="6" t="b">
         <v>0</v>
       </c>
-      <c r="U18" s="6" t="s">
-        <v>187</v>
+      <c r="U18" s="11" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="19" spans="1:21" ht="14" x14ac:dyDescent="0.15">
@@ -6432,7 +6436,7 @@
         <v>6</v>
       </c>
       <c r="H1" s="8" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="I1" s="8" t="s">
         <v>7</v>
@@ -6491,12 +6495,12 @@
         <v>1</v>
       </c>
       <c r="J2" s="6" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="3" spans="1:21" ht="14" x14ac:dyDescent="0.15">
       <c r="A3" s="6" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>21</v>
@@ -6513,7 +6517,7 @@
     </row>
     <row r="4" spans="1:21" ht="14" x14ac:dyDescent="0.15">
       <c r="A4" s="6" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>21</v>
@@ -6530,7 +6534,7 @@
     </row>
     <row r="5" spans="1:21" ht="14" x14ac:dyDescent="0.15">
       <c r="A5" s="6" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>21</v>
@@ -6564,7 +6568,7 @@
     </row>
     <row r="7" spans="1:21" ht="14" x14ac:dyDescent="0.15">
       <c r="A7" s="6" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>21</v>
@@ -6578,7 +6582,7 @@
     </row>
     <row r="8" spans="1:21" ht="14" x14ac:dyDescent="0.15">
       <c r="A8" s="6" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B8" s="6" t="s">
         <v>21</v>
@@ -6592,7 +6596,7 @@
     </row>
     <row r="9" spans="1:21" ht="14" x14ac:dyDescent="0.15">
       <c r="A9" s="6" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B9" s="6" t="s">
         <v>28</v>
@@ -6609,7 +6613,7 @@
     </row>
     <row r="10" spans="1:21" ht="14" x14ac:dyDescent="0.15">
       <c r="A10" s="6" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B10" s="6" t="s">
         <v>28</v>
@@ -6626,7 +6630,7 @@
     </row>
     <row r="11" spans="1:21" ht="14" x14ac:dyDescent="0.15">
       <c r="A11" s="6" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B11" s="6" t="s">
         <v>28</v>
@@ -6643,7 +6647,7 @@
     </row>
     <row r="12" spans="1:21" ht="14" x14ac:dyDescent="0.15">
       <c r="A12" s="6" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B12" s="6" t="s">
         <v>25</v>
@@ -6660,7 +6664,7 @@
     </row>
     <row r="13" spans="1:21" ht="14" x14ac:dyDescent="0.15">
       <c r="A13" s="6" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B13" s="6" t="s">
         <v>25</v>
@@ -6677,7 +6681,7 @@
     </row>
     <row r="14" spans="1:21" ht="14" x14ac:dyDescent="0.15">
       <c r="A14" s="6" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B14" s="6" t="s">
         <v>25</v>
@@ -6711,7 +6715,7 @@
     </row>
     <row r="16" spans="1:21" ht="14" x14ac:dyDescent="0.15">
       <c r="A16" s="6" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B16" s="6" t="s">
         <v>38</v>
@@ -6728,7 +6732,7 @@
     </row>
     <row r="17" spans="1:20" ht="14" x14ac:dyDescent="0.15">
       <c r="A17" s="6" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B17" s="6" t="s">
         <v>95</v>
@@ -6745,7 +6749,7 @@
     </row>
     <row r="18" spans="1:20" ht="14" x14ac:dyDescent="0.15">
       <c r="A18" s="6" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B18" s="6" t="s">
         <v>95</v>
@@ -6762,7 +6766,7 @@
     </row>
     <row r="19" spans="1:20" ht="14" x14ac:dyDescent="0.15">
       <c r="A19" s="6" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B19" s="6" t="s">
         <v>95</v>
@@ -6779,7 +6783,7 @@
     </row>
     <row r="20" spans="1:20" ht="14" x14ac:dyDescent="0.15">
       <c r="A20" s="6" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B20" s="6" t="s">
         <v>95</v>
@@ -6796,7 +6800,7 @@
     </row>
     <row r="21" spans="1:20" ht="14" x14ac:dyDescent="0.15">
       <c r="A21" s="6" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B21" s="6" t="s">
         <v>95</v>
@@ -6813,7 +6817,7 @@
     </row>
     <row r="22" spans="1:20" ht="14" x14ac:dyDescent="0.15">
       <c r="A22" s="6" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B22" s="6" t="s">
         <v>95</v>
@@ -6830,7 +6834,7 @@
     </row>
     <row r="23" spans="1:20" ht="14" x14ac:dyDescent="0.15">
       <c r="A23" s="6" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B23" s="6" t="s">
         <v>28</v>
@@ -6859,7 +6863,7 @@
         <v>0</v>
       </c>
       <c r="T24" s="6" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="25" spans="1:20" ht="14" x14ac:dyDescent="0.15">
@@ -6881,7 +6885,7 @@
     </row>
     <row r="26" spans="1:20" ht="14" x14ac:dyDescent="0.15">
       <c r="A26" s="6" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B26" s="6" t="s">
         <v>21</v>
@@ -6895,7 +6899,7 @@
     </row>
     <row r="27" spans="1:20" ht="14" x14ac:dyDescent="0.15">
       <c r="A27" s="6" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B27" s="6" t="s">
         <v>25</v>
@@ -6912,7 +6916,7 @@
     </row>
     <row r="28" spans="1:20" ht="14" x14ac:dyDescent="0.15">
       <c r="A28" s="6" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B28" s="6" t="s">
         <v>95</v>
@@ -6926,7 +6930,7 @@
     </row>
     <row r="29" spans="1:20" ht="14" x14ac:dyDescent="0.15">
       <c r="A29" s="6" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B29" s="6" t="s">
         <v>95</v>
@@ -6943,7 +6947,7 @@
     </row>
     <row r="30" spans="1:20" ht="14" x14ac:dyDescent="0.15">
       <c r="A30" s="6" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B30" s="6" t="s">
         <v>28</v>
@@ -6960,7 +6964,7 @@
     </row>
     <row r="31" spans="1:20" ht="14" x14ac:dyDescent="0.15">
       <c r="A31" s="6" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B31" s="6" t="s">
         <v>95</v>
@@ -6977,7 +6981,7 @@
     </row>
     <row r="32" spans="1:20" ht="14" x14ac:dyDescent="0.15">
       <c r="A32" s="6" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B32" s="6" t="s">
         <v>28</v>
@@ -6991,7 +6995,7 @@
     </row>
     <row r="33" spans="1:7" ht="14" x14ac:dyDescent="0.15">
       <c r="A33" s="6" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B33" s="6" t="s">
         <v>25</v>
@@ -7008,7 +7012,7 @@
     </row>
     <row r="34" spans="1:7" ht="14" x14ac:dyDescent="0.15">
       <c r="A34" s="6" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B34" s="6" t="s">
         <v>28</v>
@@ -7042,7 +7046,7 @@
     </row>
     <row r="36" spans="1:7" ht="14" x14ac:dyDescent="0.15">
       <c r="A36" s="6" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B36" s="6" t="s">
         <v>28</v>
@@ -7059,7 +7063,7 @@
     </row>
     <row r="37" spans="1:7" ht="14" x14ac:dyDescent="0.15">
       <c r="A37" s="6" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B37" s="6" t="s">
         <v>25</v>
@@ -7076,7 +7080,7 @@
     </row>
     <row r="38" spans="1:7" ht="14" x14ac:dyDescent="0.15">
       <c r="A38" s="6" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B38" s="6" t="s">
         <v>25</v>
@@ -7093,7 +7097,7 @@
     </row>
     <row r="39" spans="1:7" ht="14" x14ac:dyDescent="0.15">
       <c r="A39" s="6" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B39" s="6" t="s">
         <v>21</v>
@@ -7107,7 +7111,7 @@
     </row>
     <row r="40" spans="1:7" ht="14" x14ac:dyDescent="0.15">
       <c r="A40" s="6" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B40" s="6" t="s">
         <v>95</v>
@@ -7124,7 +7128,7 @@
     </row>
     <row r="41" spans="1:7" ht="14" x14ac:dyDescent="0.15">
       <c r="A41" s="6" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B41" s="6" t="s">
         <v>95</v>
@@ -7141,7 +7145,7 @@
     </row>
     <row r="42" spans="1:7" ht="14" x14ac:dyDescent="0.15">
       <c r="A42" s="6" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B42" s="6" t="s">
         <v>25</v>
@@ -7158,7 +7162,7 @@
     </row>
     <row r="43" spans="1:7" ht="14" x14ac:dyDescent="0.15">
       <c r="A43" s="6" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B43" s="6" t="s">
         <v>25</v>
@@ -7175,7 +7179,7 @@
     </row>
     <row r="44" spans="1:7" ht="14" x14ac:dyDescent="0.15">
       <c r="A44" s="6" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B44" s="6" t="s">
         <v>95</v>
@@ -7192,7 +7196,7 @@
     </row>
     <row r="45" spans="1:7" ht="14" x14ac:dyDescent="0.15">
       <c r="A45" s="6" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B45" s="6" t="s">
         <v>28</v>
@@ -7206,7 +7210,7 @@
     </row>
     <row r="46" spans="1:7" ht="14" x14ac:dyDescent="0.15">
       <c r="A46" s="6" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B46" s="6" t="s">
         <v>95</v>
@@ -7223,7 +7227,7 @@
     </row>
     <row r="47" spans="1:7" ht="14" x14ac:dyDescent="0.15">
       <c r="A47" s="6" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B47" s="6" t="s">
         <v>95</v>
@@ -7240,7 +7244,7 @@
     </row>
     <row r="48" spans="1:7" ht="14" x14ac:dyDescent="0.15">
       <c r="A48" s="6" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B48" s="6" t="s">
         <v>21</v>
@@ -7254,7 +7258,7 @@
     </row>
     <row r="49" spans="1:7" ht="14" x14ac:dyDescent="0.15">
       <c r="A49" s="6" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B49" s="6" t="s">
         <v>21</v>
@@ -7268,7 +7272,7 @@
     </row>
     <row r="50" spans="1:7" ht="14" x14ac:dyDescent="0.15">
       <c r="A50" s="6" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B50" s="6" t="s">
         <v>21</v>
@@ -7282,7 +7286,7 @@
     </row>
     <row r="51" spans="1:7" ht="14" x14ac:dyDescent="0.15">
       <c r="A51" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B51" s="6" t="s">
         <v>21</v>
@@ -7296,7 +7300,7 @@
     </row>
     <row r="52" spans="1:7" ht="14" x14ac:dyDescent="0.15">
       <c r="A52" s="6" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B52" s="6" t="s">
         <v>21</v>
@@ -7310,7 +7314,7 @@
     </row>
     <row r="53" spans="1:7" ht="14" x14ac:dyDescent="0.15">
       <c r="A53" s="6" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B53" s="6" t="s">
         <v>28</v>
@@ -7324,7 +7328,7 @@
     </row>
     <row r="54" spans="1:7" ht="14" x14ac:dyDescent="0.15">
       <c r="A54" s="6" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B54" s="6" t="s">
         <v>28</v>
@@ -7341,7 +7345,7 @@
     </row>
     <row r="55" spans="1:7" ht="14" x14ac:dyDescent="0.15">
       <c r="A55" s="6" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B55" s="6" t="s">
         <v>28</v>
@@ -7358,7 +7362,7 @@
     </row>
     <row r="56" spans="1:7" ht="14" x14ac:dyDescent="0.15">
       <c r="A56" s="6" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B56" s="6" t="s">
         <v>28</v>
@@ -7375,7 +7379,7 @@
     </row>
     <row r="57" spans="1:7" ht="14" x14ac:dyDescent="0.15">
       <c r="A57" s="6" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B57" s="6" t="s">
         <v>28</v>
@@ -7392,7 +7396,7 @@
     </row>
     <row r="58" spans="1:7" ht="14" x14ac:dyDescent="0.15">
       <c r="A58" s="6" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B58" s="6" t="s">
         <v>28</v>
@@ -7406,7 +7410,7 @@
     </row>
     <row r="59" spans="1:7" ht="14" x14ac:dyDescent="0.15">
       <c r="A59" s="6" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B59" s="6" t="s">
         <v>28</v>
@@ -7420,7 +7424,7 @@
     </row>
     <row r="60" spans="1:7" ht="14" x14ac:dyDescent="0.15">
       <c r="A60" s="6" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B60" s="6" t="s">
         <v>95</v>
@@ -7437,7 +7441,7 @@
     </row>
     <row r="61" spans="1:7" ht="14" x14ac:dyDescent="0.15">
       <c r="A61" s="6" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B61" s="6" t="s">
         <v>95</v>
@@ -7454,7 +7458,7 @@
     </row>
     <row r="62" spans="1:7" ht="14" x14ac:dyDescent="0.15">
       <c r="A62" s="6" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B62" s="6" t="s">
         <v>25</v>
@@ -7471,7 +7475,7 @@
     </row>
     <row r="63" spans="1:7" ht="14" x14ac:dyDescent="0.15">
       <c r="A63" s="6" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B63" s="6" t="s">
         <v>28</v>
@@ -7488,7 +7492,7 @@
     </row>
     <row r="64" spans="1:7" ht="14" x14ac:dyDescent="0.15">
       <c r="A64" s="6" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B64" s="6" t="s">
         <v>28</v>
@@ -7505,7 +7509,7 @@
     </row>
     <row r="65" spans="1:7" ht="14" x14ac:dyDescent="0.15">
       <c r="A65" s="6" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B65" s="6" t="s">
         <v>25</v>
@@ -7522,7 +7526,7 @@
     </row>
     <row r="66" spans="1:7" ht="14" x14ac:dyDescent="0.15">
       <c r="A66" s="6" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B66" s="6" t="s">
         <v>21</v>
@@ -7536,7 +7540,7 @@
     </row>
     <row r="67" spans="1:7" ht="14" x14ac:dyDescent="0.15">
       <c r="A67" s="6" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B67" s="6" t="s">
         <v>21</v>
@@ -7550,7 +7554,7 @@
     </row>
     <row r="68" spans="1:7" ht="14" x14ac:dyDescent="0.15">
       <c r="A68" s="6" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B68" s="6" t="s">
         <v>21</v>
@@ -7564,7 +7568,7 @@
     </row>
     <row r="69" spans="1:7" ht="14" x14ac:dyDescent="0.15">
       <c r="A69" s="6" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B69" s="6" t="s">
         <v>21</v>
@@ -7578,7 +7582,7 @@
     </row>
     <row r="70" spans="1:7" ht="14" x14ac:dyDescent="0.15">
       <c r="A70" s="6" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B70" s="6" t="s">
         <v>21</v>
@@ -7592,7 +7596,7 @@
     </row>
     <row r="71" spans="1:7" ht="14" x14ac:dyDescent="0.15">
       <c r="A71" s="6" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B71" s="6" t="s">
         <v>25</v>
@@ -7609,7 +7613,7 @@
     </row>
     <row r="72" spans="1:7" ht="14" x14ac:dyDescent="0.15">
       <c r="A72" s="6" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B72" s="6" t="s">
         <v>95</v>
@@ -7623,7 +7627,7 @@
     </row>
     <row r="73" spans="1:7" ht="14" x14ac:dyDescent="0.15">
       <c r="A73" s="6" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B73" s="6" t="s">
         <v>95</v>
@@ -7640,7 +7644,7 @@
     </row>
     <row r="74" spans="1:7" ht="14" x14ac:dyDescent="0.15">
       <c r="A74" s="6" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B74" s="6" t="s">
         <v>28</v>
@@ -7657,7 +7661,7 @@
     </row>
     <row r="75" spans="1:7" ht="14" x14ac:dyDescent="0.15">
       <c r="A75" s="6" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B75" s="6" t="s">
         <v>21</v>
@@ -7671,7 +7675,7 @@
     </row>
     <row r="76" spans="1:7" ht="14" x14ac:dyDescent="0.15">
       <c r="A76" s="6" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B76" s="6" t="s">
         <v>25</v>
@@ -7688,7 +7692,7 @@
     </row>
     <row r="77" spans="1:7" ht="14" x14ac:dyDescent="0.15">
       <c r="A77" s="6" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B77" s="6" t="s">
         <v>25</v>
@@ -7705,7 +7709,7 @@
     </row>
     <row r="78" spans="1:7" ht="14" x14ac:dyDescent="0.15">
       <c r="A78" s="6" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B78" s="6" t="s">
         <v>28</v>
@@ -7722,7 +7726,7 @@
     </row>
     <row r="79" spans="1:7" ht="14" x14ac:dyDescent="0.15">
       <c r="A79" s="6" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B79" s="6" t="s">
         <v>25</v>
@@ -7739,7 +7743,7 @@
     </row>
     <row r="80" spans="1:7" ht="14" x14ac:dyDescent="0.15">
       <c r="A80" s="6" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B80" s="6" t="s">
         <v>21</v>
@@ -7753,7 +7757,7 @@
     </row>
     <row r="81" spans="1:15" ht="14" x14ac:dyDescent="0.15">
       <c r="A81" s="6" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B81" s="6" t="s">
         <v>25</v>
@@ -7770,7 +7774,7 @@
     </row>
     <row r="82" spans="1:15" ht="14" x14ac:dyDescent="0.15">
       <c r="A82" s="6" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B82" s="6" t="s">
         <v>95</v>
@@ -7787,7 +7791,7 @@
     </row>
     <row r="83" spans="1:15" ht="14" x14ac:dyDescent="0.15">
       <c r="A83" s="6" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B83" s="6" t="s">
         <v>95</v>
@@ -7804,7 +7808,7 @@
     </row>
     <row r="84" spans="1:15" ht="14" x14ac:dyDescent="0.15">
       <c r="A84" s="6" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B84" s="6" t="s">
         <v>95</v>
@@ -7821,7 +7825,7 @@
     </row>
     <row r="85" spans="1:15" ht="14" x14ac:dyDescent="0.15">
       <c r="A85" s="6" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B85" s="6" t="s">
         <v>25</v>
@@ -7838,7 +7842,7 @@
     </row>
     <row r="86" spans="1:15" ht="14" x14ac:dyDescent="0.15">
       <c r="A86" s="6" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B86" s="6" t="s">
         <v>95</v>
@@ -7852,7 +7856,7 @@
     </row>
     <row r="87" spans="1:15" ht="14" x14ac:dyDescent="0.15">
       <c r="A87" s="6" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B87" s="6" t="s">
         <v>25</v>
@@ -7869,7 +7873,7 @@
     </row>
     <row r="88" spans="1:15" ht="14" x14ac:dyDescent="0.15">
       <c r="A88" s="6" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B88" s="6" t="s">
         <v>25</v>
@@ -7886,7 +7890,7 @@
     </row>
     <row r="89" spans="1:15" ht="14" x14ac:dyDescent="0.15">
       <c r="A89" s="6" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B89" s="6" t="s">
         <v>28</v>
@@ -7938,7 +7942,7 @@
         <v>61</v>
       </c>
       <c r="N91" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="O91" s="1" t="s">
         <v>50</v>
@@ -7964,7 +7968,7 @@
         <v>61</v>
       </c>
       <c r="N92" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="O92" s="1" t="s">
         <v>50</v>
@@ -7996,7 +8000,7 @@
     </row>
     <row r="94" spans="1:15" ht="14" x14ac:dyDescent="0.15">
       <c r="A94" s="6" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B94" s="6" t="s">
         <v>28</v>
@@ -8013,10 +8017,10 @@
     </row>
     <row r="95" spans="1:15" ht="14" x14ac:dyDescent="0.15">
       <c r="A95" s="6" t="s">
+        <v>277</v>
+      </c>
+      <c r="B95" s="6" t="s">
         <v>278</v>
-      </c>
-      <c r="B95" s="6" t="s">
-        <v>279</v>
       </c>
       <c r="F95" s="6" t="b">
         <v>1</v>
@@ -8045,7 +8049,7 @@
         <v>61</v>
       </c>
       <c r="N96" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="O96" s="1" t="s">
         <v>50</v>
@@ -8071,7 +8075,7 @@
         <v>61</v>
       </c>
       <c r="N97" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="O97" s="1" t="s">
         <v>50</v>
@@ -8105,7 +8109,7 @@
     </row>
     <row r="99" spans="1:15" ht="14" x14ac:dyDescent="0.15">
       <c r="A99" s="6" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B99" s="6" t="s">
         <v>28</v>
@@ -8139,7 +8143,7 @@
     </row>
     <row r="101" spans="1:15" ht="14" x14ac:dyDescent="0.15">
       <c r="A101" s="6" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B101" s="6" t="s">
         <v>21</v>
@@ -8153,7 +8157,7 @@
     </row>
     <row r="102" spans="1:15" ht="14" x14ac:dyDescent="0.15">
       <c r="A102" s="6" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B102" s="6" t="s">
         <v>25</v>
@@ -8170,7 +8174,7 @@
     </row>
     <row r="103" spans="1:15" ht="14" x14ac:dyDescent="0.15">
       <c r="A103" s="6" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B103" s="6" t="s">
         <v>25</v>
@@ -8187,7 +8191,7 @@
     </row>
     <row r="104" spans="1:15" ht="14" x14ac:dyDescent="0.15">
       <c r="A104" s="6" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B104" s="6" t="s">
         <v>25</v>
@@ -8204,7 +8208,7 @@
     </row>
     <row r="105" spans="1:15" ht="14" x14ac:dyDescent="0.15">
       <c r="A105" s="6" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B105" s="6" t="s">
         <v>38</v>
@@ -8221,7 +8225,7 @@
     </row>
     <row r="106" spans="1:15" ht="14" x14ac:dyDescent="0.15">
       <c r="A106" s="6" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B106" s="6" t="s">
         <v>28</v>
@@ -8238,7 +8242,7 @@
     </row>
     <row r="107" spans="1:15" ht="14" x14ac:dyDescent="0.15">
       <c r="A107" s="6" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B107" s="6" t="s">
         <v>28</v>
@@ -8258,7 +8262,7 @@
     </row>
     <row r="108" spans="1:15" ht="14" x14ac:dyDescent="0.15">
       <c r="A108" s="6" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B108" s="6" t="s">
         <v>28</v>
@@ -8275,7 +8279,7 @@
     </row>
     <row r="109" spans="1:15" ht="14" x14ac:dyDescent="0.15">
       <c r="A109" s="6" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B109" s="6" t="s">
         <v>28</v>
@@ -8306,7 +8310,7 @@
     </row>
     <row r="111" spans="1:15" ht="14" x14ac:dyDescent="0.15">
       <c r="A111" s="6" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B111" s="6" t="s">
         <v>28</v>
@@ -8347,7 +8351,7 @@
         <v>61</v>
       </c>
       <c r="N112" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="O112" s="1" t="s">
         <v>54</v>
@@ -8355,7 +8359,7 @@
     </row>
     <row r="113" spans="1:7" ht="14" x14ac:dyDescent="0.15">
       <c r="A113" s="6" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B113" s="6" t="s">
         <v>28</v>
@@ -8386,7 +8390,7 @@
     </row>
     <row r="115" spans="1:7" ht="14" x14ac:dyDescent="0.15">
       <c r="A115" s="6" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B115" s="6" t="s">
         <v>95</v>
@@ -11576,7 +11580,7 @@
         <v>6</v>
       </c>
       <c r="H1" s="8" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="I1" s="8" t="s">
         <v>7</v>
@@ -11654,7 +11658,7 @@
     </row>
     <row r="3" spans="1:21" ht="14" x14ac:dyDescent="0.15">
       <c r="A3" s="6" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>21</v>
@@ -11684,7 +11688,7 @@
     </row>
     <row r="4" spans="1:21" ht="14" x14ac:dyDescent="0.15">
       <c r="A4" s="6" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>28</v>
@@ -11773,7 +11777,7 @@
         <v>73</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="O6" s="1" t="s">
         <v>54</v>
@@ -11810,7 +11814,7 @@
         <v>73</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="O7" s="1" t="s">
         <v>32</v>
@@ -11823,7 +11827,7 @@
     </row>
     <row r="8" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="6" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B8" s="6" t="s">
         <v>28</v>
@@ -11877,7 +11881,7 @@
         <v>73</v>
       </c>
       <c r="N9" s="1" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="O9" s="1" t="s">
         <v>50</v>
@@ -11890,7 +11894,7 @@
     </row>
     <row r="10" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="6" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B10" s="6" t="s">
         <v>21</v>
@@ -11922,7 +11926,7 @@
     </row>
     <row r="11" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="6" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B11" s="6" t="s">
         <v>21</v>
@@ -11940,7 +11944,7 @@
       <c r="I11" s="6"/>
       <c r="J11" s="6"/>
       <c r="K11" s="6" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="L11" s="6"/>
       <c r="M11" s="6"/>
@@ -11954,7 +11958,7 @@
     </row>
     <row r="12" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="6" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B12" s="6" t="s">
         <v>21</v>
@@ -11972,7 +11976,7 @@
       <c r="I12" s="6"/>
       <c r="J12" s="6"/>
       <c r="K12" s="6" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="L12" s="6"/>
       <c r="M12" s="6"/>
@@ -12015,12 +12019,12 @@
       <c r="R13" s="6"/>
       <c r="T13" s="1"/>
       <c r="U13" s="1" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="14" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="6" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B14" s="6" t="s">
         <v>28</v>
@@ -13042,7 +13046,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA323256-295A-E94A-BCEC-986A220FD8FC}">
   <dimension ref="A1:U6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
@@ -13071,7 +13075,7 @@
         <v>6</v>
       </c>
       <c r="H1" s="8" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="I1" s="8" t="s">
         <v>7</v>
@@ -14435,7 +14439,7 @@
         <v>6</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="I1" s="4" t="s">
         <v>7</v>
@@ -14474,7 +14478,7 @@
         <v>186</v>
       </c>
       <c r="U1" s="10" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Make DOB into a proper date format Remove POC
</commit_message>
<xml_diff>
--- a/etl2/docs/mapping_doc.xlsx
+++ b/etl2/docs/mapping_doc.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jennifermackown/Documents/MOJ/opg-data-casrec-migration/etl2/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17B31E55-392B-BA41-B31B-196873E26B08}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F348669-41EE-B74E-B4E3-FB7CC90BC9DD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="22920" windowHeight="28340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22940" yWindow="460" windowWidth="45860" windowHeight="28340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="persons (Client)" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="900" uniqueCount="305">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="901" uniqueCount="306">
   <si>
     <t>column_name</t>
   </si>
@@ -1023,6 +1023,9 @@
   </si>
   <si>
     <t>Logdate</t>
+  </si>
+  <si>
+    <t>date_format_standard</t>
   </si>
 </sst>
 </file>
@@ -1380,9 +1383,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="U19" sqref="U19"/>
+      <selection pane="bottomLeft" activeCell="J49" sqref="J49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1531,6 +1534,9 @@
       </c>
       <c r="O5" s="6" t="s">
         <v>25</v>
+      </c>
+      <c r="T5" s="6" t="s">
+        <v>305</v>
       </c>
     </row>
     <row r="6" spans="1:21" ht="14" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
link deputy addresses removed debug stuff tidy
</commit_message>
<xml_diff>
--- a/etl2/docs/mapping_doc.xlsx
+++ b/etl2/docs/mapping_doc.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jennifermackown/Documents/MOJ/opg-data-casrec-migration/etl2/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68F74F6C-A9E4-C84C-B790-C94289CCA1AA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{519C44DC-6738-2A45-B492-BA32FB2F284C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22940" yWindow="460" windowWidth="45860" windowHeight="28340" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22940" yWindow="460" windowWidth="45860" windowHeight="28340" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="persons (Client)" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1090" uniqueCount="304">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1092" uniqueCount="305">
   <si>
     <t>column_name</t>
   </si>
@@ -1021,6 +1021,9 @@
   </si>
   <si>
     <t>Dep Adrs1,Dep Adrs2,Dep Adrs3</t>
+  </si>
+  <si>
+    <t>order</t>
   </si>
 </sst>
 </file>
@@ -1380,7 +1383,7 @@
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:XFD1048576"/>
+      <selection pane="bottomLeft" activeCell="A49" sqref="A49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -5040,7 +5043,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:U1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="N4" sqref="N4"/>
     </sheetView>
   </sheetViews>
@@ -7605,7 +7608,7 @@
   <dimension ref="A1:V1000"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="V71" sqref="V71"/>
     </sheetView>
   </sheetViews>
@@ -10000,9 +10003,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:U1000"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="T24" sqref="T24"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="U11" sqref="U11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -10224,6 +10227,9 @@
       <c r="G10" s="6" t="b">
         <v>0</v>
       </c>
+      <c r="U10" s="11" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="11" spans="1:21" ht="14" x14ac:dyDescent="0.15">
       <c r="A11" s="6" t="s">
@@ -10327,7 +10333,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:20" ht="14" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:21" ht="14" x14ac:dyDescent="0.15">
       <c r="A17" s="6" t="s">
         <v>196</v>
       </c>
@@ -10344,7 +10350,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:20" ht="14" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:21" ht="14" x14ac:dyDescent="0.15">
       <c r="A18" s="6" t="s">
         <v>197</v>
       </c>
@@ -10361,7 +10367,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:20" ht="14" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:21" ht="14" x14ac:dyDescent="0.15">
       <c r="A19" s="6" t="s">
         <v>198</v>
       </c>
@@ -10378,7 +10384,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:20" ht="14" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:21" ht="14" x14ac:dyDescent="0.15">
       <c r="A20" s="6" t="s">
         <v>199</v>
       </c>
@@ -10395,7 +10401,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:20" ht="14" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:21" ht="14" x14ac:dyDescent="0.15">
       <c r="A21" s="6" t="s">
         <v>200</v>
       </c>
@@ -10412,7 +10418,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:20" ht="14" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:21" ht="14" x14ac:dyDescent="0.15">
       <c r="A22" s="6" t="s">
         <v>201</v>
       </c>
@@ -10429,7 +10435,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:20" ht="14" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:21" ht="14" x14ac:dyDescent="0.15">
       <c r="A23" s="6" t="s">
         <v>202</v>
       </c>
@@ -10446,7 +10452,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:20" ht="14" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:21" ht="14" x14ac:dyDescent="0.15">
       <c r="A24" s="6" t="s">
         <v>40</v>
       </c>
@@ -10463,7 +10469,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="25" spans="1:20" ht="14" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:21" ht="14" x14ac:dyDescent="0.15">
       <c r="A25" s="6" t="s">
         <v>41</v>
       </c>
@@ -10479,8 +10485,11 @@
       <c r="G25" s="6" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:20" ht="14" x14ac:dyDescent="0.15">
+      <c r="U25" s="11" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="26" spans="1:21" ht="14" x14ac:dyDescent="0.15">
       <c r="A26" s="6" t="s">
         <v>203</v>
       </c>
@@ -10494,7 +10503,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:20" ht="14" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:21" ht="14" x14ac:dyDescent="0.15">
       <c r="A27" s="6" t="s">
         <v>204</v>
       </c>
@@ -10511,7 +10520,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:20" ht="14" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:21" ht="14" x14ac:dyDescent="0.15">
       <c r="A28" s="6" t="s">
         <v>205</v>
       </c>
@@ -10525,7 +10534,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:20" ht="14" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:21" ht="14" x14ac:dyDescent="0.15">
       <c r="A29" s="6" t="s">
         <v>206</v>
       </c>
@@ -10542,7 +10551,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:20" ht="14" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:21" ht="14" x14ac:dyDescent="0.15">
       <c r="A30" s="6" t="s">
         <v>207</v>
       </c>
@@ -10559,7 +10568,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:20" ht="14" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:21" ht="14" x14ac:dyDescent="0.15">
       <c r="A31" s="6" t="s">
         <v>208</v>
       </c>
@@ -10576,7 +10585,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:20" ht="14" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:21" ht="14" x14ac:dyDescent="0.15">
       <c r="A32" s="6" t="s">
         <v>209</v>
       </c>

</xml_diff>